<commit_message>
30 sept commit 2
</commit_message>
<xml_diff>
--- a/Russian Dictionary.xlsx
+++ b/Russian Dictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="541">
   <si>
     <t>Word / Expression</t>
   </si>
@@ -1011,9 +1011,6 @@
     <t>и я понимаю только немного</t>
   </si>
   <si>
-    <t>eh ya ponimayu tol'ka nemnoga</t>
-  </si>
-  <si>
     <t>do you know where's Tverskaya street is?</t>
   </si>
   <si>
@@ -1299,13 +1296,349 @@
     <t>no bez menya</t>
   </si>
   <si>
-    <t>start from lesson 6</t>
-  </si>
-  <si>
     <t>я хочу пить кое-что</t>
   </si>
   <si>
     <t>do you know where's Pushkin street Ms. Petrova?</t>
+  </si>
+  <si>
+    <t>also / too</t>
+  </si>
+  <si>
+    <t>тоже</t>
+  </si>
+  <si>
+    <t>tojah</t>
+  </si>
+  <si>
+    <t>tell me please, do you know where Pushkin street is?</t>
+  </si>
+  <si>
+    <t>скажите пожалуйста, вы знаете где пушкинская улица?</t>
+  </si>
+  <si>
+    <t>skajite pajaluysta, vy znayete gdieh Pushkinskaya olitsa?</t>
+  </si>
+  <si>
+    <t>and Red Square is here?</t>
+  </si>
+  <si>
+    <t>а красная площадь здесь?</t>
+  </si>
+  <si>
+    <t>ah krasnaya ploshchad' zdes'?</t>
+  </si>
+  <si>
+    <t>I understand well but speak only a little</t>
+  </si>
+  <si>
+    <t>я понимаю хорошо, но говорю только немного</t>
+  </si>
+  <si>
+    <t>ya ponimayu kharasho no gavaryu tolka nemnoga</t>
+  </si>
+  <si>
+    <t>yes, I want to drink (short)</t>
+  </si>
+  <si>
+    <t>да, хочу пить</t>
+  </si>
+  <si>
+    <t>dah, khatchu peet'</t>
+  </si>
+  <si>
+    <t>and not over there</t>
+  </si>
+  <si>
+    <t>e ne tam</t>
+  </si>
+  <si>
+    <t>e ya ponimayu tol'ka nemnoga</t>
+  </si>
+  <si>
+    <t>и не там</t>
+  </si>
+  <si>
+    <t>at my place</t>
+  </si>
+  <si>
+    <t>у меня</t>
+  </si>
+  <si>
+    <t>oh menya</t>
+  </si>
+  <si>
+    <t>at your place</t>
+  </si>
+  <si>
+    <t>у вас</t>
+  </si>
+  <si>
+    <t>oh vas</t>
+  </si>
+  <si>
+    <t>у вас?</t>
+  </si>
+  <si>
+    <t>oh vas?</t>
+  </si>
+  <si>
+    <t>at your place?</t>
+  </si>
+  <si>
+    <t>yes, at my place</t>
+  </si>
+  <si>
+    <t>да, у меня</t>
+  </si>
+  <si>
+    <t>dah, oh menya</t>
+  </si>
+  <si>
+    <t>ya tojah</t>
+  </si>
+  <si>
+    <t>я тоже</t>
+  </si>
+  <si>
+    <t>me too / I too</t>
+  </si>
+  <si>
+    <t>yes, at your place</t>
+  </si>
+  <si>
+    <t>да, у вас</t>
+  </si>
+  <si>
+    <t>dah, oh vas</t>
+  </si>
+  <si>
+    <t>я тоже хочу поесть</t>
+  </si>
+  <si>
+    <t>me too want to eat</t>
+  </si>
+  <si>
+    <t>ya tojah khatchu payest'</t>
+  </si>
+  <si>
+    <t>you too?</t>
+  </si>
+  <si>
+    <t>вы тоже?</t>
+  </si>
+  <si>
+    <t>vy tojah?</t>
+  </si>
+  <si>
+    <t>when?</t>
+  </si>
+  <si>
+    <t>когда?</t>
+  </si>
+  <si>
+    <t>kagda?</t>
+  </si>
+  <si>
+    <t>now</t>
+  </si>
+  <si>
+    <t>сейчас</t>
+  </si>
+  <si>
+    <t>do you want to eat?</t>
+  </si>
+  <si>
+    <t>вы хотите поесть?</t>
+  </si>
+  <si>
+    <t>vy khatite payest'?</t>
+  </si>
+  <si>
+    <t>when do you want to eat?</t>
+  </si>
+  <si>
+    <t>когда вы хотите поесть?</t>
+  </si>
+  <si>
+    <t>kagda vy khatite payest'?</t>
+  </si>
+  <si>
+    <t>when do you want to eat Mr. Gordon?</t>
+  </si>
+  <si>
+    <t>когда вы хотите поесть мистер Гордон?</t>
+  </si>
+  <si>
+    <t>kagda vy khatite payest' mister gordon?</t>
+  </si>
+  <si>
+    <t>when do you want to eat sir?</t>
+  </si>
+  <si>
+    <t>когда вы хотите поесть сэр?</t>
+  </si>
+  <si>
+    <t>kagda vy khatite payest' sir?</t>
+  </si>
+  <si>
+    <t>when do you want to eat Mrs. Gordon?</t>
+  </si>
+  <si>
+    <t>когда вы хотите поесть миссис Гордон?</t>
+  </si>
+  <si>
+    <t>kagda vy khatite payest' miss Gordon?</t>
+  </si>
+  <si>
+    <t>not now</t>
+  </si>
+  <si>
+    <t>не сейчас</t>
+  </si>
+  <si>
+    <t>seetchas</t>
+  </si>
+  <si>
+    <t>ne seetchas</t>
+  </si>
+  <si>
+    <t>maybe later</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>может быть</t>
+  </si>
+  <si>
+    <t>mojet byt'</t>
+  </si>
+  <si>
+    <t>может быть позже</t>
+  </si>
+  <si>
+    <t>mojet byt' pojjah</t>
+  </si>
+  <si>
+    <t>later</t>
+  </si>
+  <si>
+    <t>pojjah</t>
+  </si>
+  <si>
+    <t>позже</t>
+  </si>
+  <si>
+    <t>and when do you want to drink?</t>
+  </si>
+  <si>
+    <t>когда вы хотите пить?</t>
+  </si>
+  <si>
+    <t>и когда вы хотите пить?</t>
+  </si>
+  <si>
+    <t>e kagda vy khatite peet'?</t>
+  </si>
+  <si>
+    <t>where's your place?</t>
+  </si>
+  <si>
+    <t>где у вас?</t>
+  </si>
+  <si>
+    <t>gdieh oh vas?</t>
+  </si>
+  <si>
+    <t>on Pushkin street</t>
+  </si>
+  <si>
+    <t>на пушкинская улица</t>
+  </si>
+  <si>
+    <t>na Pushkinsky olitsa</t>
+  </si>
+  <si>
+    <t>not at my place?</t>
+  </si>
+  <si>
+    <t>не у меня?</t>
+  </si>
+  <si>
+    <t>ne oh menya?</t>
+  </si>
+  <si>
+    <t>me too want to drink something</t>
+  </si>
+  <si>
+    <t>я тоже хочу пить кое-что</t>
+  </si>
+  <si>
+    <t>ya tojah khatchu peet' koweh-chto</t>
+  </si>
+  <si>
+    <t>yes, me too</t>
+  </si>
+  <si>
+    <t>да, я тоже</t>
+  </si>
+  <si>
+    <t>dah, ya tojah</t>
+  </si>
+  <si>
+    <t>when do you want to drink?</t>
+  </si>
+  <si>
+    <t>kagda vy khatite peet'?</t>
+  </si>
+  <si>
+    <t>do you want to drink anything at my place?</t>
+  </si>
+  <si>
+    <t>вы хотите пить что-нибудь у меня?</t>
+  </si>
+  <si>
+    <t>vy khatite peet' chto-nibud' oh menya?</t>
+  </si>
+  <si>
+    <t>yes, with pleasure</t>
+  </si>
+  <si>
+    <t>да, с удовольствием</t>
+  </si>
+  <si>
+    <t>I too want to eat later</t>
+  </si>
+  <si>
+    <t>я тоже хочу поесть позже</t>
+  </si>
+  <si>
+    <t>ya tojah khatchu payest' pojjah</t>
+  </si>
+  <si>
+    <t>at your place on Pushkin street?</t>
+  </si>
+  <si>
+    <t>у вас на пушкинская улица?</t>
+  </si>
+  <si>
+    <t>oh vas na Pushkinsky olitsa?</t>
+  </si>
+  <si>
+    <t>with pleasure</t>
+  </si>
+  <si>
+    <t>da, s udah vol'st viyem</t>
+  </si>
+  <si>
+    <t>s udah vol'st viyem</t>
+  </si>
+  <si>
+    <t>с удовольствием</t>
+  </si>
+  <si>
+    <t>start at unit 7</t>
   </si>
 </sst>
 </file>
@@ -1353,7 +1686,277 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1801,11 +2404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D145"/>
+  <dimension ref="B1:D182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,7 +3635,7 @@
         <v>330</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>331</v>
+        <v>445</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>329</v>
@@ -3040,57 +3643,57 @@
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>337</v>
-      </c>
       <c r="D113" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D114" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
@@ -3101,356 +3704,826 @@
         <v>325</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="D119" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D121" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="D122" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="D123" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>367</v>
-      </c>
       <c r="D124" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="D126" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="D127" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="D129" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="D130" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C131" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="D131" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="D132" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>393</v>
-      </c>
       <c r="D134" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="D137" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>403</v>
-      </c>
       <c r="D138" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D139" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="D142" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C143" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>423</v>
-      </c>
       <c r="D143" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="D144" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="1" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B44 D45 B46:B101 B103:B106 B108:B123 B125:B126 B131:B132 B134 B137 B143:B1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  <conditionalFormatting sqref="B1:B44 D45 B46:B101 B103:B106 B108:B123 B125:B126 B131:B132 B134 B137 B143:B147 B150:B152 B158:B160 D154 B168:B169 B172 B175 B178 B180:B1048576">
+    <cfRule type="duplicateValues" dxfId="41" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B107">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B127">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B128">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B129">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B130">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B133">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B138">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B139">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B142">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B148">
+    <cfRule type="duplicateValues" dxfId="26" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B149">
+    <cfRule type="duplicateValues" dxfId="25" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B153">
+    <cfRule type="duplicateValues" dxfId="24" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B154">
+    <cfRule type="duplicateValues" dxfId="23" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B155">
+    <cfRule type="duplicateValues" dxfId="22" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B156">
+    <cfRule type="duplicateValues" dxfId="21" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B157">
+    <cfRule type="duplicateValues" dxfId="20" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B161">
+    <cfRule type="duplicateValues" dxfId="19" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B162">
+    <cfRule type="duplicateValues" dxfId="18" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B163">
+    <cfRule type="duplicateValues" dxfId="17" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B164">
+    <cfRule type="duplicateValues" dxfId="16" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B165">
+    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B166">
+    <cfRule type="duplicateValues" dxfId="14" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B167">
+    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B170">
+    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B171">
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B173">
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B174">
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B176">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B177">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B179">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>